<commit_message>
Block for one flip while in the screen
</commit_message>
<xml_diff>
--- a/extras/example_form/Coin_flip.xlsx
+++ b/extras/example_form/Coin_flip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehrab Ali\Documents\GitHub\coinflip\extras\example_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD0D6C4-D1D0-409A-9D78-71FC5EB60DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0061B-5047-4A00-AED3-363B1F4254FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="396">
   <si>
     <t>type</t>
   </si>
@@ -2571,6 +2571,12 @@
   </si>
   <si>
     <t>coin_flip_sample</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${coin})</t>
   </si>
 </sst>
 </file>
@@ -4916,11 +4922,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5130,6 +5136,9 @@
       </c>
     </row>
     <row r="13" spans="1:23">
+      <c r="B13" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="G13"/>
       <c r="H13"/>
       <c r="K13"/>
@@ -5183,68 +5192,65 @@
         <v>133</v>
       </c>
       <c r="B16" s="92" t="s">
+        <v>394</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="92" t="s">
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B18" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N18" s="9" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="92" t="s">
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B19" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="N19" s="9" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="47.25">
-      <c r="A19" s="92" t="s">
+    <row r="20" spans="1:14" ht="47.25">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B20" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -5252,6 +5258,20 @@
         <v>362</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>362</v>
       </c>
     </row>
@@ -5548,7 +5568,7 @@
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2209161408</v>
+        <v>2209161945</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>362</v>

</xml_diff>

<commit_message>
Store the random number
</commit_message>
<xml_diff>
--- a/extras/example_form/Coin_flip.xlsx
+++ b/extras/example_form/Coin_flip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehrab Ali\Documents\GitHub\coinflip\extras\example_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0061B-5047-4A00-AED3-363B1F4254FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240F067D-F00C-461F-9DAF-1BA99005D57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2558,15 +2558,9 @@
     <t>item-at('|', plug-in-metadata(${coin}), 1)</t>
   </si>
   <si>
-    <t>item-at('|', plug-in-metadata(${coin}), ${flipcount})</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>count-items('|', plug-in-metadata(${coin}))-1</t>
-  </si>
-  <si>
     <t>Coin Flip Example</t>
   </si>
   <si>
@@ -2577,6 +2571,12 @@
   </si>
   <si>
     <t>plug-in-metadata(${coin})</t>
+  </si>
+  <si>
+    <t>item-at('|', plug-in-metadata(${coin}), count-items('|', plug-in-metadata(${coin})))</t>
+  </si>
+  <si>
+    <t>(count-items('|', plug-in-metadata(${coin})) - 1) div 2</t>
   </si>
 </sst>
 </file>
@@ -3048,7 +3048,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3287,7 +3287,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4926,7 +4925,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5188,14 +5187,14 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="92" t="s">
-        <v>394</v>
+      <c r="B16" s="2" t="s">
+        <v>392</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -5206,7 +5205,7 @@
         <v>383</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -5228,7 +5227,7 @@
         <v>385</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="47.25">
@@ -5264,7 +5263,7 @@
         <v>362</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -5561,14 +5560,14 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2209161945</v>
+        <v>2209162049</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>362</v>

</xml_diff>

<commit_message>
Change to real coin
</commit_message>
<xml_diff>
--- a/extras/example_form/Coin_flip.xlsx
+++ b/extras/example_form/Coin_flip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehrab Ali\Documents\GitHub\coinflip\extras\example_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBD01F2-15DC-48F8-B81D-CAF10C919102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B152A1F-6362-4FEF-B36E-36A63A03DDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="400">
   <si>
     <t>type</t>
   </si>
@@ -4935,9 +4935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5542,10 +5542,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2209192236</v>
+        <v>2209301129</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>362</v>
@@ -5602,6 +5602,14 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="D5" t="s">
         <v>377</v>
       </c>
     </row>

</xml_diff>